<commit_message>
Reorganise the folder and rename some files.
</commit_message>
<xml_diff>
--- a/data/data_syntax_us.xlsx
+++ b/data/data_syntax_us.xlsx
@@ -1,29 +1,30 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="27715"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10609"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ChiaraSantolin/Desktop/PostDoc/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/GonzaloGGC/projects/flip/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{32842990-8F0D-F848-B169-7CCE61C2CAF6}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="700" yWindow="460" windowWidth="25600" windowHeight="13960"/>
+    <workbookView xWindow="700" yWindow="460" windowWidth="25600" windowHeight="13960" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="150001" concurrentCalc="0"/>
+  <calcPr calcId="150001"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
     </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+      <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
-    </ext>
-    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
-      <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
 </workbook>
@@ -86,7 +87,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -431,19 +432,20 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J34"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A21" sqref="A21:XFD21"/>
+    <sheetView tabSelected="1" zoomScale="84" workbookViewId="0">
+      <selection activeCell="J4" sqref="J4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="3" max="3" width="10.6640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.6640625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10.6640625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="9.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.83203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.83203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.83203125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.2">

</xml_diff>